<commit_message>
-Changing some issues in the design to improve the performance
</commit_message>
<xml_diff>
--- a/H21R20/Released/BOM/H21R20.xlsx
+++ b/H21R20/Released/BOM/H21R20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H21R20\H21R20\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBAAC4C9-0A66-4CFD-B8C7-C47CA34B5B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492E3221-5290-4F69-9C96-EF0DE1E94F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="98">
   <si>
     <t>Description</t>
   </si>
@@ -172,18 +172,6 @@
     <t>https://octopart.com/mmz1608y300bta00-tdk-7906990?r=sp</t>
   </si>
   <si>
-    <t>Transistor, Bipolar, Si, NPN, General Purpose, VCEO 40VDC, IC 200mA, PD 225mW, SOT-23</t>
-  </si>
-  <si>
-    <t>ON Semiconductor</t>
-  </si>
-  <si>
-    <t>MMBT3904LT1G</t>
-  </si>
-  <si>
-    <t>https://octopart.com/mmbt3904lt1g-on+semiconductor-3280?r=sp</t>
-  </si>
-  <si>
     <t>STM32G0B1CEU6N</t>
   </si>
   <si>
@@ -238,12 +226,6 @@
     <t>Hexabitz Modules</t>
   </si>
   <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>C1, C5 , C7 , C4, C12</t>
-  </si>
-  <si>
     <t>C13</t>
   </si>
   <si>
@@ -262,15 +244,9 @@
     <t>C10 , C11</t>
   </si>
   <si>
-    <t>C6 , C9</t>
-  </si>
-  <si>
     <t>R3 , R8 , R9 , R11 ,R12 ,R13</t>
   </si>
   <si>
-    <t>R2 , R5 , R7 , R10 , R14 ,R15</t>
-  </si>
-  <si>
     <t>R1 , R4</t>
   </si>
   <si>
@@ -335,6 +311,15 @@
   </si>
   <si>
     <t xml:space="preserve">ESP32-C3 Wifi+BLE (H21R20) </t>
+  </si>
+  <si>
+    <t>C1,C2, C5 , C7 , C4, C12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R2 , R5 , R7 , R10 , R14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C6 </t>
   </si>
 </sst>
 </file>
@@ -988,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G26"/>
+  <dimension ref="A2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1022,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
@@ -1048,7 +1033,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
@@ -1065,7 +1050,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1137,7 +1122,7 @@
     </row>
     <row r="11" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>35</v>
@@ -1157,19 +1142,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F12" s="17">
         <v>2</v>
@@ -1177,10 +1162,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>39</v>
@@ -1197,10 +1182,10 @@
     </row>
     <row r="14" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>41</v>
@@ -1212,24 +1197,24 @@
         <v>42</v>
       </c>
       <c r="F14" s="17">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F15" s="17">
         <v>2</v>
@@ -1237,10 +1222,10 @@
     </row>
     <row r="16" spans="1:7" ht="24" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>30</v>
@@ -1252,15 +1237,15 @@
         <v>31</v>
       </c>
       <c r="F16" s="17">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>33</v>
@@ -1272,15 +1257,15 @@
         <v>34</v>
       </c>
       <c r="F17" s="17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>18</v>
@@ -1297,19 +1282,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="F19" s="17">
         <v>1</v>
@@ -1337,19 +1322,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F21" s="17">
         <v>2</v>
@@ -1357,19 +1342,19 @@
     </row>
     <row r="22" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F22" s="17">
         <v>8</v>
@@ -1377,81 +1362,61 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="B23" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>50</v>
-      </c>
       <c r="D23" s="15" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F23" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>53</v>
+      <c r="A24" s="20" t="s">
+        <v>78</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>52</v>
+        <v>79</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>55</v>
+        <v>80</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="F24" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
-        <v>86</v>
+      <c r="A25" s="15" t="s">
+        <v>55</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>89</v>
+        <v>56</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
       <c r="F25" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1469,17 +1434,16 @@
     <hyperlink ref="E11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="E14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="E20" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E24" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E26" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E25" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E23" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E12" r:id="rId14" xr:uid="{C5EFCC27-D3E0-42E3-8BC5-671D4233CA12}"/>
-    <hyperlink ref="E22" r:id="rId15" xr:uid="{C48DC70B-AEDD-4B55-8F2A-2E283523F27E}"/>
+    <hyperlink ref="E12" r:id="rId13" xr:uid="{C5EFCC27-D3E0-42E3-8BC5-671D4233CA12}"/>
+    <hyperlink ref="E22" r:id="rId14" xr:uid="{C48DC70B-AEDD-4B55-8F2A-2E283523F27E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>
-  <drawing r:id="rId17"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId15"/>
+  <drawing r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Improve the layout design -Change the jumber resistors footprint to 0402
</commit_message>
<xml_diff>
--- a/H21R20/Released/BOM/H21R20.xlsx
+++ b/H21R20/Released/BOM/H21R20.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\OneDrive\Documents\H21R2x-Hardware\H21R20\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H21R2x-Hardware\H21R20\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC0FF2D-C342-48D4-A499-2C18083BDF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164C07C2-243B-49B0-BC21-732CD20CBB4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H21R00" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="97">
   <si>
     <t>Description</t>
   </si>
@@ -94,18 +94,9 @@
     <t>JP1</t>
   </si>
   <si>
-    <t>PCB Header, Unshrouded, Thru 02 Straight Header, .101, AMPMODU Mod II Series</t>
-  </si>
-  <si>
     <t>TE Connectivity</t>
   </si>
   <si>
-    <t>87227-1</t>
-  </si>
-  <si>
-    <t>https://octopart.com/87227-1-te+connectivity-39512052?r=sp</t>
-  </si>
-  <si>
     <t>JP2</t>
   </si>
   <si>
@@ -124,27 +115,12 @@
     <t>https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g</t>
   </si>
   <si>
-    <t>YAGEO [VA]</t>
-  </si>
-  <si>
     <t>CC0805KKX7R7BB105</t>
   </si>
   <si>
     <t>https://octopart.com/cc0805kkx7r7bb105-yageo-8376555?r=sp</t>
   </si>
   <si>
-    <t>RES SMD 0.0OHM JUMPER 1/10W 0603</t>
-  </si>
-  <si>
-    <t>YAGEO [VR]</t>
-  </si>
-  <si>
-    <t>RC0603JR-070RL</t>
-  </si>
-  <si>
-    <t>https://octopart.com/rc0603jr-070rl-yageo-1241539?r=sp</t>
-  </si>
-  <si>
     <t>ERJ-3GEYJ271V</t>
   </si>
   <si>
@@ -320,17 +296,38 @@
   </si>
   <si>
     <t xml:space="preserve">C6 </t>
+  </si>
+  <si>
+    <t>RES SMD 0 OHM JUMPER 1/16W 0402</t>
+  </si>
+  <si>
+    <t>AC0402JR-070RL</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>Headers &amp; Wire Housings Unshrouded 1 POS T/H</t>
+  </si>
+  <si>
+    <t>5-146280-1</t>
+  </si>
+  <si>
+    <t>https://octopart.com/5-146280-1-te+connectivity+%2F+amp-40259676?r=sp</t>
+  </si>
+  <si>
+    <t>https://octopart.com/ac0402jr-070rl-yageo-21711084?r=sp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -338,7 +335,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -349,34 +346,28 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="28"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -397,7 +388,7 @@
     <font>
       <b/>
       <sz val="36"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -518,7 +509,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -526,53 +517,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -593,9 +586,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -634,7 +624,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>2174599</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>20002</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -974,43 +964,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="84" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" customWidth="1"/>
+    <col min="2" max="2" width="55.09765625" customWidth="1"/>
+    <col min="3" max="3" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.09765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="46.2" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:7" ht="45.6" x14ac:dyDescent="0.75">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1027,12 +1016,12 @@
       <c r="F4" s="20"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
@@ -1044,12 +1033,12 @@
       <c r="F5" s="23"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1059,17 +1048,17 @@
       <c r="F6" s="26"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="3" t="s">
@@ -1079,343 +1068,343 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="E9" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="16" t="s">
+      <c r="C10" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="17">
+      <c r="D10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="15" t="s">
+    <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F11" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="D16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="16" t="s">
+      <c r="F16" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="17">
+      <c r="D17" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="F12" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B14" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="17">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="F15" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="17">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="17">
+      <c r="E24" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>90</v>
-      </c>
-      <c r="F19" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="16" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+      <c r="B25" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="D25" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="17">
+      <c r="F25" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1427,22 +1416,20 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E17" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E18" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E11" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E14" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E20" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E23" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E25" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E13" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E12" r:id="rId13" xr:uid="{C5EFCC27-D3E0-42E3-8BC5-671D4233CA12}"/>
-    <hyperlink ref="E22" r:id="rId14" xr:uid="{C48DC70B-AEDD-4B55-8F2A-2E283523F27E}"/>
+    <hyperlink ref="E17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E20" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E23" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E21" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E25" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{C5EFCC27-D3E0-42E3-8BC5-671D4233CA12}"/>
+    <hyperlink ref="E22" r:id="rId12" xr:uid="{C48DC70B-AEDD-4B55-8F2A-2E283523F27E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId15"/>
-  <drawing r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId13"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>